<commit_message>
add colors t xlsx
</commit_message>
<xml_diff>
--- a/dev_qa_image_tags_compare.xlsx
+++ b/dev_qa_image_tags_compare.xlsx
@@ -29,12 +29,30 @@
       <b val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FF00"/>
+        <bgColor rgb="0000FF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FF0000"/>
+        <bgColor rgb="00FF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFFF00"/>
+        <bgColor rgb="00FFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -55,11 +73,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -466,7 +487,7 @@
           <t>cart-checkout</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>cart-calculation-api.yaml</t>
         </is>
@@ -481,7 +502,7 @@
           <t>release-2023-12-294-gd549d9965</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
+      <c r="E2" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -493,22 +514,22 @@
           <t>cart-checkout</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>slots-indexer.yaml</t>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>order-workflow-service.yaml</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>0.1.7-1-g87ca86b</t>
+          <t>0.1.33-2-ge477d6c</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>0.1.7-1-g87ca86b</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
+          <t>0.1.33-2-ge477d6c</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -520,24 +541,24 @@
           <t>cart-checkout</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>order-workflow-service.yaml</t>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>order-router.yaml</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>0.1.33-2-ge477d6c</t>
+          <t>v1.0.2-69-ge754cb3</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>0.1.33-2-ge477d6c</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Match</t>
+          <t>v1.0.2-89-ga38a381</t>
+        </is>
+      </c>
+      <c r="E4" s="3" t="inlineStr">
+        <is>
+          <t>Dev &lt; QA</t>
         </is>
       </c>
     </row>
@@ -547,24 +568,24 @@
           <t>cart-checkout</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>orderprogress-invoice-sender.yaml</t>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>cart-checkout-utility.yaml</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>v2.1.17-86-g3d8529e</t>
+          <t>0.0.2-3-g4f1692f</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>v2.1.17-86-g3d8529e</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Match</t>
+          <t>0.0.3-rc</t>
+        </is>
+      </c>
+      <c r="E5" s="3" t="inlineStr">
+        <is>
+          <t>Dev &lt; QA</t>
         </is>
       </c>
     </row>
@@ -574,22 +595,22 @@
           <t>cart-checkout</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>cart-checkout-utility.yaml</t>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>orderprogress-api.yaml</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>0.0.2-3-g4f1692f</t>
+          <t>v2.2.9-126-g6fc91ee</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>0.0.3-rc</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
+          <t>v2.2.9-92-g3903c77</t>
+        </is>
+      </c>
+      <c r="E6" s="3" t="inlineStr">
         <is>
           <t>Dev &lt; QA</t>
         </is>
@@ -601,7 +622,7 @@
           <t>cart-checkout</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>cart-rewards-api.yaml</t>
         </is>
@@ -616,7 +637,7 @@
           <t>v1.0.42-79-g611d69c</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
+      <c r="E7" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -628,24 +649,24 @@
           <t>cart-checkout</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>orderprogress-api.yaml</t>
+      <c r="B8" s="2" t="inlineStr">
+        <is>
+          <t>orderstatus-worker.yaml</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>v2.2.9-126-g6fc91ee</t>
+          <t>v2.1.15-43-gd89a742</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>v2.2.9-92-g3903c77</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Dev &lt; QA</t>
+          <t>v2.1.15-43-gd89a742</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>Match</t>
         </is>
       </c>
     </row>
@@ -655,22 +676,22 @@
           <t>cart-checkout</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>orderstatus-worker.yaml</t>
+      <c r="B9" s="2" t="inlineStr">
+        <is>
+          <t>slots-indexer.yaml</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>v2.1.15-43-gd89a742</t>
+          <t>0.1.7-1-g87ca86b</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>v2.1.15-43-gd89a742</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
+          <t>0.1.7-1-g87ca86b</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -682,24 +703,24 @@
           <t>cart-checkout</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>order-router.yaml</t>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>slots-api.yaml</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>v1.0.2-69-ge754cb3</t>
+          <t>v1.2.40-125-g8d4d9eb</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>v1.0.2-89-ga38a381</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Dev &lt; QA</t>
+          <t>v1.2.40-125-g8d4d9eb</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>Match</t>
         </is>
       </c>
     </row>
@@ -709,22 +730,22 @@
           <t>cart-checkout</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>slots-api.yaml</t>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>order-streaming.yaml</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>v1.2.40-125-g8d4d9eb</t>
+          <t>1.3.4-2-g71a8e11</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>v1.2.40-125-g8d4d9eb</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
+          <t>1.3.4-2-g71a8e11</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -736,22 +757,22 @@
           <t>cart-checkout</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>order-streaming.yaml</t>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>orderprogress-invoice-sender.yaml</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>1.3.4-2-g71a8e11</t>
+          <t>v2.1.17-86-g3d8529e</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>1.3.4-2-g71a8e11</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
+          <t>v2.1.17-86-g3d8529e</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -763,24 +784,24 @@
           <t>data-integration</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>store-api.yaml</t>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>app-config-api.yaml</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>1.0.1-4-gd7809f2</t>
+          <t>1.1.26-28-g9782bc1</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>1.0.0-3-g4fd527a</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Dev &gt; QA</t>
+          <t>1.1.26-7-g93d69d0</t>
+        </is>
+      </c>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>Dev &lt; QA</t>
         </is>
       </c>
     </row>
@@ -790,22 +811,22 @@
           <t>data-integration</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>product-info-api.yaml</t>
+      <c r="B14" s="2" t="inlineStr">
+        <is>
+          <t>product-category-api.yaml</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>0.1.0-2-g388dc64</t>
+          <t>1.0.0-rc</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>0.1.0-2-g388dc64</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
+          <t>1.0.0-rc</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -817,7 +838,7 @@
           <t>data-integration</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="B15" s="2" t="inlineStr">
         <is>
           <t>product-admin.yaml</t>
         </is>
@@ -832,7 +853,7 @@
           <t>v1.0.25-77-gbed1e18</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E15" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -844,24 +865,24 @@
           <t>data-integration</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>past-purchase.yaml</t>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>coupon-check-ui.yaml</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>3.0.1-rc</t>
+          <t>1.2.29-34-g2f23ee6e</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>3.0.1-rc</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Match</t>
+          <t>v1.1.5-42-gcedb5dec</t>
+        </is>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>Dev &lt; QA</t>
         </is>
       </c>
     </row>
@@ -871,22 +892,22 @@
           <t>data-integration</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>product-category-api.yaml</t>
+      <c r="B17" s="2" t="inlineStr">
+        <is>
+          <t>past-purchase.yaml</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>1.0.0-rc</t>
+          <t>3.0.1-rc</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>1.0.0-rc</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
+          <t>3.0.1-rc</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -898,22 +919,22 @@
           <t>data-integration</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>store-locator.yaml</t>
+      <c r="B18" s="4" t="inlineStr">
+        <is>
+          <t>store-api.yaml</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>2.0.0-9-gd736484</t>
+          <t>1.0.1-4-gd7809f2</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>2.0.0-1-gc5a25f1</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
+          <t>1.0.0-3-g4fd527a</t>
+        </is>
+      </c>
+      <c r="E18" s="4" t="inlineStr">
         <is>
           <t>Dev &gt; QA</t>
         </is>
@@ -925,22 +946,22 @@
           <t>data-integration</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>job-api.yaml</t>
+      <c r="B19" s="4" t="inlineStr">
+        <is>
+          <t>store-locator.yaml</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>v1.0.6.bkp.before.2023.3.0-53-g39d1085</t>
+          <t>2.0.0-9-gd736484</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>v1.0.6.bkp.before.2023.3.0-36-ge0093f3</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
+          <t>2.0.0-1-gc5a25f1</t>
+        </is>
+      </c>
+      <c r="E19" s="4" t="inlineStr">
         <is>
           <t>Dev &gt; QA</t>
         </is>
@@ -952,24 +973,24 @@
           <t>data-integration</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>coupon-check-ui.yaml</t>
+      <c r="B20" s="2" t="inlineStr">
+        <is>
+          <t>product-info-api.yaml</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>1.2.29-34-g2f23ee6e</t>
+          <t>0.1.0-2-g388dc64</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>v1.1.5-42-gcedb5dec</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Dev &lt; QA</t>
+          <t>0.1.0-2-g388dc64</t>
+        </is>
+      </c>
+      <c r="E20" s="2" t="inlineStr">
+        <is>
+          <t>Match</t>
         </is>
       </c>
     </row>
@@ -979,24 +1000,24 @@
           <t>data-integration</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>app-config-api.yaml</t>
+      <c r="B21" s="4" t="inlineStr">
+        <is>
+          <t>job-api.yaml</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>1.1.26-28-g9782bc1</t>
+          <t>v1.0.6.bkp.before.2023.3.0-53-g39d1085</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>1.1.26-7-g93d69d0</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Dev &lt; QA</t>
+          <t>v1.0.6.bkp.before.2023.3.0-36-ge0093f3</t>
+        </is>
+      </c>
+      <c r="E21" s="4" t="inlineStr">
+        <is>
+          <t>Dev &gt; QA</t>
         </is>
       </c>
     </row>
@@ -1006,22 +1027,22 @@
           <t>customer-customer</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>external-domain-api.yaml</t>
+      <c r="B22" s="2" t="inlineStr">
+        <is>
+          <t>legacy-data-api.yaml</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>v0.0.4-82-g8b3fc9c</t>
+          <t>1.0.14-8-g806fa30</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>v0.0.4-82-g8b3fc9c</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
+          <t>1.0.14-8-g806fa30</t>
+        </is>
+      </c>
+      <c r="E22" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1033,22 +1054,22 @@
           <t>customer-customer</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>subscription-manager-api.yaml</t>
+      <c r="B23" s="2" t="inlineStr">
+        <is>
+          <t>external-domain-api.yaml</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>v0.0.16-178-gf44f19c</t>
+          <t>v0.0.4-82-g8b3fc9c</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>v0.0.16-178-gf44f19c</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
+          <t>v0.0.4-82-g8b3fc9c</t>
+        </is>
+      </c>
+      <c r="E23" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1060,22 +1081,22 @@
           <t>customer-customer</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>device-notification-api.yaml</t>
+      <c r="B24" s="2" t="inlineStr">
+        <is>
+          <t>external-domain-router.yaml</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>v1.1.4-64-ged97bdf</t>
+          <t>v1.0.2-69-ge754cb3</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>v1.1.4-64-ged97bdf</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
+          <t>v1.0.2-69-ge754cb3</t>
+        </is>
+      </c>
+      <c r="E24" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1087,24 +1108,24 @@
           <t>customer-customer</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>device-sms-api.yaml</t>
+      <c r="B25" s="3" t="inlineStr">
+        <is>
+          <t>profile-api.yaml</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>v1.2.9-53-gd1922c7</t>
+          <t>v1.5.2-847-g2f78dcda</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>v1.2.9-53-gd1922c7</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Match</t>
+          <t>v1.5.2-959-g410e7e5d</t>
+        </is>
+      </c>
+      <c r="E25" s="3" t="inlineStr">
+        <is>
+          <t>Dev &lt; QA</t>
         </is>
       </c>
     </row>
@@ -1114,24 +1135,24 @@
           <t>customer-customer</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>notification-api.yaml</t>
+      <c r="B26" s="2" t="inlineStr">
+        <is>
+          <t>id-generator-service.yaml</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>1.x.x-4-g76a6a15</t>
+          <t>1.x.x-1-g5850171</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>1.x.x-7-g67ffb0b</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Dev &lt; QA</t>
+          <t>1.x.x-1-g5850171</t>
+        </is>
+      </c>
+      <c r="E26" s="2" t="inlineStr">
+        <is>
+          <t>Match</t>
         </is>
       </c>
     </row>
@@ -1141,22 +1162,22 @@
           <t>customer-customer</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>profile-api.yaml</t>
+      <c r="B27" s="3" t="inlineStr">
+        <is>
+          <t>notification-api.yaml</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>v1.5.2-847-g2f78dcda</t>
+          <t>1.x.x-4-g76a6a15</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>v1.5.2-959-g410e7e5d</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
+          <t>1.x.x-7-g67ffb0b</t>
+        </is>
+      </c>
+      <c r="E27" s="3" t="inlineStr">
         <is>
           <t>Dev &lt; QA</t>
         </is>
@@ -1168,7 +1189,7 @@
           <t>customer-customer</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="B28" s="2" t="inlineStr">
         <is>
           <t>profile-router.yaml</t>
         </is>
@@ -1183,7 +1204,7 @@
           <t>v1.0.2-69-ge754cb3</t>
         </is>
       </c>
-      <c r="E28" t="inlineStr">
+      <c r="E28" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1195,22 +1216,22 @@
           <t>customer-customer</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>template-engine-handler-router.yaml</t>
+      <c r="B29" s="2" t="inlineStr">
+        <is>
+          <t>template-engine-handler.yaml</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>v1.0.2-69-ge754cb3</t>
+          <t>v1.0.6-53-g08fbc4c</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>v1.0.2-69-ge754cb3</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
+          <t>v1.0.6-53-g08fbc4c</t>
+        </is>
+      </c>
+      <c r="E29" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1222,22 +1243,22 @@
           <t>customer-customer</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>legacy-data-api.yaml</t>
+      <c r="B30" s="2" t="inlineStr">
+        <is>
+          <t>jwt-authorization-server.yaml</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>1.0.14-8-g806fa30</t>
+          <t>v1.0.1-75-g8bea82f</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>1.0.14-8-g806fa30</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
+          <t>v1.0.1-75-g8bea82f</t>
+        </is>
+      </c>
+      <c r="E30" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1249,24 +1270,24 @@
           <t>customer-customer</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>session-management-api.yaml</t>
+      <c r="B31" s="2" t="inlineStr">
+        <is>
+          <t>device-notification-api.yaml</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>v1.10.5-273-g0967ee7</t>
+          <t>v1.1.4-64-ged97bdf</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>v1.10.5-329-ge99d28d</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>Dev &lt; QA</t>
+          <t>v1.1.4-64-ged97bdf</t>
+        </is>
+      </c>
+      <c r="E31" s="2" t="inlineStr">
+        <is>
+          <t>Match</t>
         </is>
       </c>
     </row>
@@ -1276,22 +1297,22 @@
           <t>customer-customer</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>device-data-api.yaml</t>
+      <c r="B32" s="2" t="inlineStr">
+        <is>
+          <t>device-sms-api.yaml</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>1.x.x-6-gf64a124</t>
+          <t>v1.2.9-53-gd1922c7</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>1.x.x-6-gf64a124</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
+          <t>v1.2.9-53-gd1922c7</t>
+        </is>
+      </c>
+      <c r="E32" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1303,24 +1324,24 @@
           <t>customer-customer</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>jwt-authorization-server.yaml</t>
+      <c r="B33" s="3" t="inlineStr">
+        <is>
+          <t>session-management-api.yaml</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>v1.0.1-75-g8bea82f</t>
+          <t>v1.10.5-273-g0967ee7</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>v1.0.1-75-g8bea82f</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>Match</t>
+          <t>v1.10.5-329-ge99d28d</t>
+        </is>
+      </c>
+      <c r="E33" s="3" t="inlineStr">
+        <is>
+          <t>Dev &lt; QA</t>
         </is>
       </c>
     </row>
@@ -1330,9 +1351,9 @@
           <t>customer-customer</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>external-domain-router.yaml</t>
+      <c r="B34" s="2" t="inlineStr">
+        <is>
+          <t>template-engine-handler-router.yaml</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
@@ -1345,7 +1366,7 @@
           <t>v1.0.2-69-ge754cb3</t>
         </is>
       </c>
-      <c r="E34" t="inlineStr">
+      <c r="E34" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1357,22 +1378,22 @@
           <t>customer-customer</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>id-generator-service.yaml</t>
+      <c r="B35" s="2" t="inlineStr">
+        <is>
+          <t>device-data-api.yaml</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>1.x.x-1-g5850171</t>
+          <t>1.x.x-6-gf64a124</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>1.x.x-1-g5850171</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
+          <t>1.x.x-6-gf64a124</t>
+        </is>
+      </c>
+      <c r="E35" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1384,22 +1405,22 @@
           <t>customer-customer</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>template-engine-handler.yaml</t>
+      <c r="B36" s="2" t="inlineStr">
+        <is>
+          <t>subscription-manager-api.yaml</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>v1.0.6-53-g08fbc4c</t>
+          <t>v0.0.16-178-gf44f19c</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>v1.0.6-53-g08fbc4c</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
+          <t>v0.0.16-178-gf44f19c</t>
+        </is>
+      </c>
+      <c r="E36" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1411,7 +1432,7 @@
           <t>payment-payment</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="B37" s="2" t="inlineStr">
         <is>
           <t>payment-service-api.yaml</t>
         </is>
@@ -1426,7 +1447,7 @@
           <t>v0.4.12-98-g9da8729</t>
         </is>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="E37" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1438,7 +1459,7 @@
           <t>payment-payment</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="B38" s="4" t="inlineStr">
         <is>
           <t>wallet-session-service.yaml</t>
         </is>
@@ -1453,7 +1474,7 @@
           <t>2.0.0-8-g4f0862a</t>
         </is>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="E38" s="4" t="inlineStr">
         <is>
           <t>Dev &gt; QA</t>
         </is>
@@ -1465,7 +1486,7 @@
           <t>oms-order-management</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="B39" s="2" t="inlineStr">
         <is>
           <t>fulfillment-router.yaml</t>
         </is>
@@ -1480,7 +1501,7 @@
           <t>v1.0.2-69-ge754cb3</t>
         </is>
       </c>
-      <c r="E39" t="inlineStr">
+      <c r="E39" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1492,24 +1513,24 @@
           <t>customer-loyalty</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>rewards-history-router.yaml</t>
+      <c r="B40" s="3" t="inlineStr">
+        <is>
+          <t>passbook.yaml</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>v1.0.2-69-ge754cb3</t>
+          <t>2.0.1-rc-10-g0723aed</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>v1.0.2-69-ge754cb3</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>Match</t>
+          <t>2.0.1-rc-2-gc516163</t>
+        </is>
+      </c>
+      <c r="E40" s="3" t="inlineStr">
+        <is>
+          <t>Dev &lt; QA</t>
         </is>
       </c>
     </row>
@@ -1519,7 +1540,7 @@
           <t>customer-loyalty</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="B41" s="4" t="inlineStr">
         <is>
           <t>contact-us.yaml</t>
         </is>
@@ -1534,7 +1555,7 @@
           <t>2.0.0-24-g10c925a</t>
         </is>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="E41" s="4" t="inlineStr">
         <is>
           <t>Dev &gt; QA</t>
         </is>
@@ -1546,22 +1567,22 @@
           <t>customer-loyalty</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>loyalty-account.yaml</t>
+      <c r="B42" s="2" t="inlineStr">
+        <is>
+          <t>product-recalls.yaml</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>1.x.x-7-g2875210</t>
+          <t>2.0.4-rc</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>1.x.x-7-g2875210</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
+          <t>2.0.4-rc</t>
+        </is>
+      </c>
+      <c r="E42" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1573,22 +1594,22 @@
           <t>customer-loyalty</t>
         </is>
       </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>product-recalls.yaml</t>
+      <c r="B43" s="2" t="inlineStr">
+        <is>
+          <t>rewards-history.yaml</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>2.0.4-rc</t>
+          <t>1.0.13-13-g7140e4b</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>2.0.4-rc</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
+          <t>1.0.13-13-g7140e4b</t>
+        </is>
+      </c>
+      <c r="E43" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1600,7 +1621,7 @@
           <t>customer-loyalty</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B44" s="2" t="inlineStr">
         <is>
           <t>rewards.yaml</t>
         </is>
@@ -1615,7 +1636,7 @@
           <t>v1.7.9-139-gb7eee7ed</t>
         </is>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="E44" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1627,24 +1648,24 @@
           <t>customer-loyalty</t>
         </is>
       </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>passbook.yaml</t>
+      <c r="B45" s="4" t="inlineStr">
+        <is>
+          <t>site-transition.yaml</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>2.0.1-rc-10-g0723aed</t>
+          <t>1.x.x-39-g43ead5e</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>2.0.1-rc-2-gc516163</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>Dev &lt; QA</t>
+          <t>1.x.x-11-g1cbaa8d</t>
+        </is>
+      </c>
+      <c r="E45" s="4" t="inlineStr">
+        <is>
+          <t>Dev &gt; QA</t>
         </is>
       </c>
     </row>
@@ -1654,22 +1675,22 @@
           <t>customer-loyalty</t>
         </is>
       </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>balances.yaml</t>
+      <c r="B46" s="2" t="inlineStr">
+        <is>
+          <t>loyalty-account.yaml</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>1.5.0-104-ga7d84ad</t>
+          <t>1.x.x-7-g2875210</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>1.5.0-104-ga7d84ad</t>
-        </is>
-      </c>
-      <c r="E46" t="inlineStr">
+          <t>1.x.x-7-g2875210</t>
+        </is>
+      </c>
+      <c r="E46" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1681,24 +1702,24 @@
           <t>customer-loyalty</t>
         </is>
       </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>site-transition.yaml</t>
+      <c r="B47" s="2" t="inlineStr">
+        <is>
+          <t>rewards-history-router.yaml</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>1.x.x-39-g43ead5e</t>
+          <t>v1.0.2-69-ge754cb3</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>1.x.x-11-g1cbaa8d</t>
-        </is>
-      </c>
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>Dev &gt; QA</t>
+          <t>v1.0.2-69-ge754cb3</t>
+        </is>
+      </c>
+      <c r="E47" s="2" t="inlineStr">
+        <is>
+          <t>Match</t>
         </is>
       </c>
     </row>
@@ -1708,22 +1729,22 @@
           <t>customer-loyalty</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>rewards-history.yaml</t>
+      <c r="B48" s="2" t="inlineStr">
+        <is>
+          <t>balances.yaml</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>1.0.13-13-g7140e4b</t>
+          <t>1.5.0-104-ga7d84ad</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>1.0.13-13-g7140e4b</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
+          <t>1.5.0-104-ga7d84ad</t>
+        </is>
+      </c>
+      <c r="E48" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1735,22 +1756,22 @@
           <t>web-frontend</t>
         </is>
       </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>entrypoint.yaml</t>
+      <c r="B49" s="2" t="inlineStr">
+        <is>
+          <t>peapod-email-service.yaml</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Not Found</t>
+          <t>0.1.80-29-g8342797</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>Not Found</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
+          <t>0.1.80-29-g8342797</t>
+        </is>
+      </c>
+      <c r="E49" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1762,7 +1783,7 @@
           <t>web-frontend</t>
         </is>
       </c>
-      <c r="B50" t="inlineStr">
+      <c r="B50" s="3" t="inlineStr">
         <is>
           <t>mail-relay-decorator.yaml</t>
         </is>
@@ -1777,7 +1798,7 @@
           <t>v2.0.16-116-g66a4ef4</t>
         </is>
       </c>
-      <c r="E50" t="inlineStr">
+      <c r="E50" s="3" t="inlineStr">
         <is>
           <t>Dev &lt; QA</t>
         </is>
@@ -1789,22 +1810,22 @@
           <t>web-frontend</t>
         </is>
       </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>peapod-email-service.yaml</t>
+      <c r="B51" s="2" t="inlineStr">
+        <is>
+          <t>entrypoint.yaml</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>0.1.80-29-g8342797</t>
+          <t>Not Found</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>0.1.80-29-g8342797</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
+          <t>Not Found</t>
+        </is>
+      </c>
+      <c r="E51" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1816,22 +1837,22 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>site-config-loader.yaml</t>
+      <c r="B52" s="2" t="inlineStr">
+        <is>
+          <t>store-router.yaml</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>v5.1.0-1139-gfe02df4</t>
+          <t>v1.0.2-69-ge754cb3</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>v5.1.0-1139-gfe02df4</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
+          <t>v1.0.2-69-ge754cb3</t>
+        </is>
+      </c>
+      <c r="E52" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1843,22 +1864,22 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>peapod-client-template-engine.yaml</t>
+      <c r="B53" s="4" t="inlineStr">
+        <is>
+          <t>pdl-router.yaml</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>v5.1.0-8975-g7edee2e535</t>
+          <t>v1.0.67-121-g4332a98</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>v5.1.0-8646-g275998622d</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
+          <t>v1.0.67-119-gf05bc01</t>
+        </is>
+      </c>
+      <c r="E53" s="4" t="inlineStr">
         <is>
           <t>Dev &gt; QA</t>
         </is>
@@ -1870,22 +1891,22 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>coupons.yaml</t>
+      <c r="B54" s="2" t="inlineStr">
+        <is>
+          <t>targeting-publisher.yaml</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>v1.4.12-166-g82f28a9</t>
+          <t>1.3.8-2-gbd9af93</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>v1.4.12-166-g82f28a9</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
+          <t>1.3.8-2-gbd9af93</t>
+        </is>
+      </c>
+      <c r="E54" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1897,22 +1918,22 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>site-config-api.yaml</t>
+      <c r="B55" s="2" t="inlineStr">
+        <is>
+          <t>coupon-api.yaml</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>v3.2.1-21-g1a2e870</t>
+          <t>v1.9.25-173-g822f672</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>v3.2.1-21-g1a2e870</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
+          <t>v1.9.25-173-g822f672</t>
+        </is>
+      </c>
+      <c r="E55" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -1924,24 +1945,24 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>personalization-router.yaml</t>
+      <c r="B56" s="4" t="inlineStr">
+        <is>
+          <t>peapod-client-template-engine.yaml</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>v1.0.2-69-ge754cb3</t>
+          <t>v5.1.0-8975-g7edee2e535</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>v1.0.2-69-ge754cb3</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>Match</t>
+          <t>v5.1.0-8646-g275998622d</t>
+        </is>
+      </c>
+      <c r="E56" s="4" t="inlineStr">
+        <is>
+          <t>Dev &gt; QA</t>
         </is>
       </c>
     </row>
@@ -1951,24 +1972,24 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>coupon-compilation-api.yaml</t>
+      <c r="B57" s="4" t="inlineStr">
+        <is>
+          <t>product-api.yaml</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>0.1.2-12-g6d197e0</t>
+          <t>v1.1.13-785-g3726438b</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>0.1.2-6-g9365747</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>Dev &lt; QA</t>
+          <t>v1.1.13-778-g849f9334</t>
+        </is>
+      </c>
+      <c r="E57" s="4" t="inlineStr">
+        <is>
+          <t>Dev &gt; QA</t>
         </is>
       </c>
     </row>
@@ -1978,22 +1999,22 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>shoppinglist-api.yaml</t>
+      <c r="B58" s="2" t="inlineStr">
+        <is>
+          <t>site-config-api.yaml</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>v1.2.3-231-gfd57fb7</t>
+          <t>v3.2.1-21-g1a2e870</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
         <is>
-          <t>v1.2.3-231-gfd57fb7</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
+          <t>v3.2.1-21-g1a2e870</t>
+        </is>
+      </c>
+      <c r="E58" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -2005,24 +2026,24 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>coupon-retrieval-api.yaml</t>
+      <c r="B59" s="2" t="inlineStr">
+        <is>
+          <t>targeting-api.yaml</t>
         </is>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>0.2.0-19-g26d2976</t>
+          <t>v1.0.20-434-gccfe67b</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
         <is>
-          <t>0.2.0-2-g2048b87</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>Dev &lt; QA</t>
+          <t>v1.0.20-434-gccfe67b</t>
+        </is>
+      </c>
+      <c r="E59" s="2" t="inlineStr">
+        <is>
+          <t>Match</t>
         </is>
       </c>
     </row>
@@ -2032,7 +2053,7 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B60" t="inlineStr">
+      <c r="B60" s="2" t="inlineStr">
         <is>
           <t>user-coupon-service.yaml</t>
         </is>
@@ -2047,7 +2068,7 @@
           <t>v1.0.44-517-ge64e716e</t>
         </is>
       </c>
-      <c r="E60" t="inlineStr">
+      <c r="E60" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -2059,22 +2080,22 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>user-coupon-router.yaml</t>
+      <c r="B61" s="2" t="inlineStr">
+        <is>
+          <t>coupons.yaml</t>
         </is>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>v1.0.2-69-ge754cb3</t>
+          <t>v1.4.12-166-g82f28a9</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
         <is>
-          <t>v1.0.2-69-ge754cb3</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
+          <t>v1.4.12-166-g82f28a9</t>
+        </is>
+      </c>
+      <c r="E61" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -2086,22 +2107,22 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>pdl-router.yaml</t>
+      <c r="B62" s="4" t="inlineStr">
+        <is>
+          <t>peapod-client-template-engine-static.yaml</t>
         </is>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>v1.0.67-121-g4332a98</t>
+          <t>v5.1.0-8975-g7edee2e535</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>v1.0.67-119-gf05bc01</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
+          <t>v5.1.0-8646-g275998622d</t>
+        </is>
+      </c>
+      <c r="E62" s="4" t="inlineStr">
         <is>
           <t>Dev &gt; QA</t>
         </is>
@@ -2113,24 +2134,24 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>targeting-api.yaml</t>
+      <c r="B63" s="4" t="inlineStr">
+        <is>
+          <t>weekly-ad-api.yaml</t>
         </is>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>v1.0.20-434-gccfe67b</t>
+          <t>1.0.0-3-gcf2ae26</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>v1.0.20-434-gccfe67b</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>Match</t>
+          <t>0.0.1-162-g6a1adc5</t>
+        </is>
+      </c>
+      <c r="E63" s="4" t="inlineStr">
+        <is>
+          <t>Dev &gt; QA</t>
         </is>
       </c>
     </row>
@@ -2140,24 +2161,24 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>weekly-ad-api.yaml</t>
+      <c r="B64" s="2" t="inlineStr">
+        <is>
+          <t>user-coupon-router.yaml</t>
         </is>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>1.0.0-3-gcf2ae26</t>
+          <t>v1.0.2-69-ge754cb3</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
         <is>
-          <t>0.0.1-162-g6a1adc5</t>
-        </is>
-      </c>
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>Dev &gt; QA</t>
+          <t>v1.0.2-69-ge754cb3</t>
+        </is>
+      </c>
+      <c r="E64" s="2" t="inlineStr">
+        <is>
+          <t>Match</t>
         </is>
       </c>
     </row>
@@ -2167,24 +2188,24 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>product-api.yaml</t>
+      <c r="B65" s="2" t="inlineStr">
+        <is>
+          <t>shoppinglist-api.yaml</t>
         </is>
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>v1.1.13-785-g3726438b</t>
+          <t>v1.2.3-231-gfd57fb7</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>v1.1.13-778-g849f9334</t>
-        </is>
-      </c>
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>Dev &gt; QA</t>
+          <t>v1.2.3-231-gfd57fb7</t>
+        </is>
+      </c>
+      <c r="E65" s="2" t="inlineStr">
+        <is>
+          <t>Match</t>
         </is>
       </c>
     </row>
@@ -2194,22 +2215,22 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>targeting-publisher.yaml</t>
+      <c r="B66" s="2" t="inlineStr">
+        <is>
+          <t>personalization-router.yaml</t>
         </is>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>1.3.8-2-gbd9af93</t>
+          <t>v1.0.2-69-ge754cb3</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>1.3.8-2-gbd9af93</t>
-        </is>
-      </c>
-      <c r="E66" t="inlineStr">
+          <t>v1.0.2-69-ge754cb3</t>
+        </is>
+      </c>
+      <c r="E66" s="2" t="inlineStr">
         <is>
           <t>Match</t>
         </is>
@@ -2221,24 +2242,24 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>peapod-client-template-engine-static.yaml</t>
+      <c r="B67" s="3" t="inlineStr">
+        <is>
+          <t>content-publisher.yaml</t>
         </is>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>v5.1.0-8975-g7edee2e535</t>
+          <t>1.x.x-138-g83867db</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>v5.1.0-8646-g275998622d</t>
-        </is>
-      </c>
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>Dev &gt; QA</t>
+          <t>1.x.x-18-gb1c071c</t>
+        </is>
+      </c>
+      <c r="E67" s="3" t="inlineStr">
+        <is>
+          <t>Dev &lt; QA</t>
         </is>
       </c>
     </row>
@@ -2248,22 +2269,22 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>seo-pages.yaml</t>
+      <c r="B68" s="4" t="inlineStr">
+        <is>
+          <t>targeting-compilation-api.yaml</t>
         </is>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>0.1.3-39-g5b9052f</t>
+          <t>1.4.4-49-g20be4e8</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>0.1.3-12-g15f3c9e</t>
-        </is>
-      </c>
-      <c r="E68" t="inlineStr">
+          <t>1.4.4-2-gc2ce593</t>
+        </is>
+      </c>
+      <c r="E68" s="4" t="inlineStr">
         <is>
           <t>Dev &gt; QA</t>
         </is>
@@ -2275,24 +2296,24 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>product-api-router.yaml</t>
+      <c r="B69" s="3" t="inlineStr">
+        <is>
+          <t>coupon-retrieval-api.yaml</t>
         </is>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>v1.0.2-69-ge754cb3</t>
+          <t>0.2.0-19-g26d2976</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>v1.0.2-69-ge754cb3</t>
-        </is>
-      </c>
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>Match</t>
+          <t>0.2.0-2-g2048b87</t>
+        </is>
+      </c>
+      <c r="E69" s="3" t="inlineStr">
+        <is>
+          <t>Dev &lt; QA</t>
         </is>
       </c>
     </row>
@@ -2302,24 +2323,24 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>content-service.yaml</t>
+      <c r="B70" s="3" t="inlineStr">
+        <is>
+          <t>coupon-compilation-api.yaml</t>
         </is>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>v1.0.5-146-g9cbc171</t>
+          <t>0.1.2-12-g6d197e0</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>v1.0.5-123-g7241ee8</t>
-        </is>
-      </c>
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>Dev &gt; QA</t>
+          <t>0.1.2-6-g9365747</t>
+        </is>
+      </c>
+      <c r="E70" s="3" t="inlineStr">
+        <is>
+          <t>Dev &lt; QA</t>
         </is>
       </c>
     </row>
@@ -2329,24 +2350,24 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>coupon-api.yaml</t>
+      <c r="B71" s="4" t="inlineStr">
+        <is>
+          <t>content-service.yaml</t>
         </is>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>v1.9.25-173-g822f672</t>
+          <t>v1.0.5-146-g9cbc171</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>v1.9.25-173-g822f672</t>
-        </is>
-      </c>
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>Match</t>
+          <t>v1.0.5-123-g7241ee8</t>
+        </is>
+      </c>
+      <c r="E71" s="4" t="inlineStr">
+        <is>
+          <t>Dev &gt; QA</t>
         </is>
       </c>
     </row>
@@ -2356,24 +2377,24 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>content-publisher.yaml</t>
+      <c r="B72" s="2" t="inlineStr">
+        <is>
+          <t>site-config-loader.yaml</t>
         </is>
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>1.x.x-138-g83867db</t>
+          <t>v5.1.0-1139-gfe02df4</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>1.x.x-18-gb1c071c</t>
-        </is>
-      </c>
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>Dev &lt; QA</t>
+          <t>v5.1.0-1139-gfe02df4</t>
+        </is>
+      </c>
+      <c r="E72" s="2" t="inlineStr">
+        <is>
+          <t>Match</t>
         </is>
       </c>
     </row>
@@ -2383,24 +2404,24 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>store-router.yaml</t>
+      <c r="B73" s="4" t="inlineStr">
+        <is>
+          <t>elasticsearch-query-router.yaml</t>
         </is>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>v1.0.2-69-ge754cb3</t>
+          <t>v1.2.2-76-g4d74dda</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
         <is>
-          <t>v1.0.2-69-ge754cb3</t>
-        </is>
-      </c>
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>Match</t>
+          <t>v1.2.2-64-g1c76b14</t>
+        </is>
+      </c>
+      <c r="E73" s="4" t="inlineStr">
+        <is>
+          <t>Dev &gt; QA</t>
         </is>
       </c>
     </row>
@@ -2410,24 +2431,24 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>elasticsearch-query-router.yaml</t>
+      <c r="B74" s="2" t="inlineStr">
+        <is>
+          <t>product-api-router.yaml</t>
         </is>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>v1.2.2-76-g4d74dda</t>
+          <t>v1.0.2-69-ge754cb3</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
         <is>
-          <t>v1.2.2-64-g1c76b14</t>
-        </is>
-      </c>
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>Dev &gt; QA</t>
+          <t>v1.0.2-69-ge754cb3</t>
+        </is>
+      </c>
+      <c r="E74" s="2" t="inlineStr">
+        <is>
+          <t>Match</t>
         </is>
       </c>
     </row>
@@ -2437,22 +2458,22 @@
           <t>search-and-browse</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>targeting-compilation-api.yaml</t>
+      <c r="B75" s="4" t="inlineStr">
+        <is>
+          <t>seo-pages.yaml</t>
         </is>
       </c>
       <c r="C75" t="inlineStr">
         <is>
-          <t>1.4.4-49-g20be4e8</t>
+          <t>0.1.3-39-g5b9052f</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
         <is>
-          <t>1.4.4-2-gc2ce593</t>
-        </is>
-      </c>
-      <c r="E75" t="inlineStr">
+          <t>0.1.3-12-g15f3c9e</t>
+        </is>
+      </c>
+      <c r="E75" s="4" t="inlineStr">
         <is>
           <t>Dev &gt; QA</t>
         </is>

</xml_diff>